<commit_message>
mod4_dom - PROMPT _dom dla test_log_giecia
</commit_message>
<xml_diff>
--- a/testy_logiki_gięcia2/2.test_wyciagania_odcinkow/archiwum/wyniki_odcinki1.0.3.xlsx
+++ b/testy_logiki_gięcia2/2.test_wyciagania_odcinkow/archiwum/wyniki_odcinki1.0.3.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PYTHON\PROJEKT_GEOMETRIA_GIĘCIA\testy_logiki_gięcia2\2.test_wyciagania_odcinkow\archiwum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2EC87E-3E3D-4A5D-B891-759852DA2A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E4BBA1-5967-48F1-967F-505830E91D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$225</definedName>
@@ -143,12 +144,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -178,16 +185,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -486,11 +503,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:M225"/>
+  <dimension ref="A1:M226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K135" sqref="K135:K139"/>
+      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K226" sqref="K226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4356,7 +4373,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>25</v>
       </c>
@@ -4496,7 +4513,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>25</v>
       </c>
@@ -4636,7 +4653,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>25</v>
       </c>
@@ -4776,7 +4793,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>25</v>
       </c>
@@ -4916,7 +4933,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>25</v>
       </c>
@@ -5056,7 +5073,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>25</v>
       </c>
@@ -5196,7 +5213,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>25</v>
       </c>
@@ -5336,7 +5353,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>25</v>
       </c>
@@ -6561,1134 +6578,1134 @@
         <v>5.9949089999999998</v>
       </c>
     </row>
-    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A174" t="s">
+    <row r="174" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B174" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C174" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D174">
+      <c r="D174" s="2">
         <v>1</v>
       </c>
-      <c r="E174">
-        <v>0</v>
-      </c>
-      <c r="F174">
+      <c r="E174" s="2">
+        <v>0</v>
+      </c>
+      <c r="F174" s="2">
         <v>138</v>
       </c>
-      <c r="G174">
-        <v>200</v>
-      </c>
-      <c r="H174">
+      <c r="G174" s="2">
+        <v>200</v>
+      </c>
+      <c r="H174" s="2">
         <v>138</v>
       </c>
-      <c r="I174" t="b">
-        <v>0</v>
-      </c>
-      <c r="J174">
-        <v>200</v>
-      </c>
-      <c r="K174">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A175" t="s">
+      <c r="I174" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J174" s="2">
+        <v>200</v>
+      </c>
+      <c r="K174" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C175" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D175">
+      <c r="D175" s="2">
         <v>2</v>
       </c>
-      <c r="E175">
-        <v>200</v>
-      </c>
-      <c r="F175">
+      <c r="E175" s="2">
+        <v>200</v>
+      </c>
+      <c r="F175" s="2">
         <v>138</v>
       </c>
-      <c r="G175">
-        <v>200</v>
-      </c>
-      <c r="H175">
-        <v>200</v>
-      </c>
-      <c r="I175" t="b">
-        <v>0</v>
-      </c>
-      <c r="J175">
+      <c r="G175" s="2">
+        <v>200</v>
+      </c>
+      <c r="H175" s="2">
+        <v>200</v>
+      </c>
+      <c r="I175" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J175" s="2">
         <v>62</v>
       </c>
-      <c r="K175">
+      <c r="K175" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A176" t="s">
+    <row r="176" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B176" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C176" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D176">
+      <c r="D176" s="2">
         <v>3</v>
       </c>
-      <c r="E176">
-        <v>200</v>
-      </c>
-      <c r="F176">
-        <v>200</v>
-      </c>
-      <c r="G176">
-        <v>0</v>
-      </c>
-      <c r="H176">
-        <v>200</v>
-      </c>
-      <c r="I176" t="b">
-        <v>0</v>
-      </c>
-      <c r="J176">
-        <v>200</v>
-      </c>
-      <c r="K176">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A177" t="s">
+      <c r="E176" s="2">
+        <v>200</v>
+      </c>
+      <c r="F176" s="2">
+        <v>200</v>
+      </c>
+      <c r="G176" s="2">
+        <v>0</v>
+      </c>
+      <c r="H176" s="2">
+        <v>200</v>
+      </c>
+      <c r="I176" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J176" s="2">
+        <v>200</v>
+      </c>
+      <c r="K176" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C177" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D177">
+      <c r="D177" s="2">
         <v>4</v>
       </c>
-      <c r="E177">
-        <v>0</v>
-      </c>
-      <c r="F177">
-        <v>200</v>
-      </c>
-      <c r="G177">
-        <v>0</v>
-      </c>
-      <c r="H177">
+      <c r="E177" s="2">
+        <v>0</v>
+      </c>
+      <c r="F177" s="2">
+        <v>200</v>
+      </c>
+      <c r="G177" s="2">
+        <v>0</v>
+      </c>
+      <c r="H177" s="2">
         <v>138</v>
       </c>
-      <c r="I177" t="b">
-        <v>0</v>
-      </c>
-      <c r="J177">
+      <c r="I177" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J177" s="2">
         <v>62</v>
       </c>
-      <c r="K177">
+      <c r="K177" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A178" t="s">
+    <row r="178" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C178" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D178">
+      <c r="D178" s="2">
         <v>1</v>
       </c>
-      <c r="E178">
-        <v>200</v>
-      </c>
-      <c r="F178">
+      <c r="E178" s="2">
+        <v>200</v>
+      </c>
+      <c r="F178" s="2">
         <v>138</v>
       </c>
-      <c r="G178">
-        <v>0</v>
-      </c>
-      <c r="H178">
+      <c r="G178" s="2">
+        <v>0</v>
+      </c>
+      <c r="H178" s="2">
         <v>138</v>
       </c>
-      <c r="I178" t="b">
-        <v>0</v>
-      </c>
-      <c r="J178">
-        <v>200</v>
-      </c>
-      <c r="K178">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A179" t="s">
+      <c r="I178" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J178" s="2">
+        <v>200</v>
+      </c>
+      <c r="K178" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B179" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C179" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D179">
+      <c r="D179" s="2">
         <v>2</v>
       </c>
-      <c r="E179">
-        <v>0</v>
-      </c>
-      <c r="F179">
+      <c r="E179" s="2">
+        <v>0</v>
+      </c>
+      <c r="F179" s="2">
         <v>138</v>
       </c>
-      <c r="G179">
-        <v>0</v>
-      </c>
-      <c r="H179">
+      <c r="G179" s="2">
+        <v>0</v>
+      </c>
+      <c r="H179" s="2">
         <v>130</v>
       </c>
-      <c r="I179" t="b">
-        <v>0</v>
-      </c>
-      <c r="J179">
+      <c r="I179" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J179" s="2">
         <v>8</v>
       </c>
-      <c r="K179">
+      <c r="K179" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
+    <row r="180" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D180">
+      <c r="D180" s="2">
         <v>3</v>
       </c>
-      <c r="E180">
-        <v>0</v>
-      </c>
-      <c r="F180">
+      <c r="E180" s="2">
+        <v>0</v>
+      </c>
+      <c r="F180" s="2">
         <v>130</v>
       </c>
-      <c r="G180">
-        <v>200</v>
-      </c>
-      <c r="H180">
+      <c r="G180" s="2">
+        <v>200</v>
+      </c>
+      <c r="H180" s="2">
         <v>130</v>
       </c>
-      <c r="I180" t="b">
-        <v>0</v>
-      </c>
-      <c r="J180">
-        <v>200</v>
-      </c>
-      <c r="K180">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A181" t="s">
+      <c r="I180" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J180" s="2">
+        <v>200</v>
+      </c>
+      <c r="K180" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C181" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D181">
+      <c r="D181" s="2">
         <v>4</v>
       </c>
-      <c r="E181">
-        <v>200</v>
-      </c>
-      <c r="F181">
+      <c r="E181" s="2">
+        <v>200</v>
+      </c>
+      <c r="F181" s="2">
         <v>130</v>
       </c>
-      <c r="G181">
-        <v>200</v>
-      </c>
-      <c r="H181">
+      <c r="G181" s="2">
+        <v>200</v>
+      </c>
+      <c r="H181" s="2">
         <v>138</v>
       </c>
-      <c r="I181" t="b">
-        <v>0</v>
-      </c>
-      <c r="J181">
+      <c r="I181" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J181" s="2">
         <v>8</v>
       </c>
-      <c r="K181">
+      <c r="K181" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A182" t="s">
+    <row r="182" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B182" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C182" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D182">
+      <c r="D182" s="2">
         <v>1</v>
       </c>
-      <c r="E182">
+      <c r="E182" s="2">
         <v>8</v>
       </c>
-      <c r="F182">
-        <v>200</v>
-      </c>
-      <c r="G182">
+      <c r="F182" s="2">
+        <v>200</v>
+      </c>
+      <c r="G182" s="2">
         <v>8</v>
       </c>
-      <c r="H182">
-        <v>0</v>
-      </c>
-      <c r="I182" t="b">
-        <v>0</v>
-      </c>
-      <c r="J182">
-        <v>200</v>
-      </c>
-      <c r="K182">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="183" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A183" t="s">
+      <c r="H182" s="2">
+        <v>0</v>
+      </c>
+      <c r="I182" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J182" s="2">
+        <v>200</v>
+      </c>
+      <c r="K182" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B183" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C183" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D183">
+      <c r="D183" s="2">
         <v>2</v>
       </c>
-      <c r="E183">
+      <c r="E183" s="2">
         <v>8</v>
       </c>
-      <c r="F183">
-        <v>0</v>
-      </c>
-      <c r="G183">
+      <c r="F183" s="2">
+        <v>0</v>
+      </c>
+      <c r="G183" s="2">
         <v>49.957273999999998</v>
       </c>
-      <c r="H183">
-        <v>0</v>
-      </c>
-      <c r="I183" t="b">
-        <v>0</v>
-      </c>
-      <c r="J183">
+      <c r="H183" s="2">
+        <v>0</v>
+      </c>
+      <c r="I183" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J183" s="2">
         <v>41.957273999999998</v>
       </c>
-      <c r="K183">
+      <c r="K183" s="2">
         <v>41.957273999999998</v>
       </c>
     </row>
-    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A184" t="s">
+    <row r="184" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C184" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D184">
+      <c r="D184" s="2">
         <v>3</v>
       </c>
-      <c r="E184">
+      <c r="E184" s="2">
         <v>49.957273999999998</v>
       </c>
-      <c r="F184">
-        <v>0</v>
-      </c>
-      <c r="G184">
+      <c r="F184" s="2">
+        <v>0</v>
+      </c>
+      <c r="G184" s="2">
         <v>49.957273999999998</v>
       </c>
-      <c r="H184">
-        <v>200</v>
-      </c>
-      <c r="I184" t="b">
-        <v>0</v>
-      </c>
-      <c r="J184">
-        <v>200</v>
-      </c>
-      <c r="K184">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A185" t="s">
+      <c r="H184" s="2">
+        <v>200</v>
+      </c>
+      <c r="I184" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J184" s="2">
+        <v>200</v>
+      </c>
+      <c r="K184" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B185" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C185" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D185">
+      <c r="D185" s="2">
         <v>4</v>
       </c>
-      <c r="E185">
+      <c r="E185" s="2">
         <v>49.957273999999998</v>
       </c>
-      <c r="F185">
-        <v>200</v>
-      </c>
-      <c r="G185">
+      <c r="F185" s="2">
+        <v>200</v>
+      </c>
+      <c r="G185" s="2">
         <v>8</v>
       </c>
-      <c r="H185">
-        <v>200</v>
-      </c>
-      <c r="I185" t="b">
-        <v>0</v>
-      </c>
-      <c r="J185">
+      <c r="H185" s="2">
+        <v>200</v>
+      </c>
+      <c r="I185" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J185" s="2">
         <v>41.957273999999998</v>
       </c>
-      <c r="K185">
+      <c r="K185" s="2">
         <v>41.957273999999998</v>
       </c>
     </row>
-    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
+    <row r="186" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B186" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C186" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D186">
+      <c r="D186" s="2">
         <v>1</v>
       </c>
-      <c r="E186">
+      <c r="E186" s="2">
         <v>49.957273999999998</v>
       </c>
-      <c r="F186">
-        <v>200</v>
-      </c>
-      <c r="G186">
+      <c r="F186" s="2">
+        <v>200</v>
+      </c>
+      <c r="G186" s="2">
         <v>49.957273999999998</v>
       </c>
-      <c r="H186">
-        <v>0</v>
-      </c>
-      <c r="I186" t="b">
-        <v>0</v>
-      </c>
-      <c r="J186">
-        <v>200</v>
-      </c>
-      <c r="K186">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A187" t="s">
+      <c r="H186" s="2">
+        <v>0</v>
+      </c>
+      <c r="I186" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J186" s="2">
+        <v>200</v>
+      </c>
+      <c r="K186" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C187" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D187">
+      <c r="D187" s="2">
         <v>2</v>
       </c>
-      <c r="E187">
+      <c r="E187" s="2">
         <v>49.957273999999998</v>
       </c>
-      <c r="F187">
-        <v>0</v>
-      </c>
-      <c r="G187">
+      <c r="F187" s="2">
+        <v>0</v>
+      </c>
+      <c r="G187" s="2">
         <v>60</v>
       </c>
-      <c r="H187">
-        <v>0</v>
-      </c>
-      <c r="I187" t="b">
-        <v>0</v>
-      </c>
-      <c r="J187">
+      <c r="H187" s="2">
+        <v>0</v>
+      </c>
+      <c r="I187" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J187" s="2">
         <v>10.042726</v>
       </c>
-      <c r="K187">
+      <c r="K187" s="2">
         <v>10.042726</v>
       </c>
     </row>
-    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
+    <row r="188" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C188" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D188">
+      <c r="D188" s="2">
         <v>3</v>
       </c>
-      <c r="E188">
+      <c r="E188" s="2">
         <v>60</v>
       </c>
-      <c r="F188">
-        <v>0</v>
-      </c>
-      <c r="G188">
+      <c r="F188" s="2">
+        <v>0</v>
+      </c>
+      <c r="G188" s="2">
         <v>60</v>
       </c>
-      <c r="H188">
-        <v>200</v>
-      </c>
-      <c r="I188" t="b">
-        <v>0</v>
-      </c>
-      <c r="J188">
-        <v>200</v>
-      </c>
-      <c r="K188">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A189" t="s">
+      <c r="H188" s="2">
+        <v>200</v>
+      </c>
+      <c r="I188" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J188" s="2">
+        <v>200</v>
+      </c>
+      <c r="K188" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B189" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C189" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D189">
+      <c r="D189" s="2">
         <v>4</v>
       </c>
-      <c r="E189">
+      <c r="E189" s="2">
         <v>60</v>
       </c>
-      <c r="F189">
-        <v>200</v>
-      </c>
-      <c r="G189">
+      <c r="F189" s="2">
+        <v>200</v>
+      </c>
+      <c r="G189" s="2">
         <v>49.957273999999998</v>
       </c>
-      <c r="H189">
-        <v>200</v>
-      </c>
-      <c r="I189" t="b">
-        <v>0</v>
-      </c>
-      <c r="J189">
+      <c r="H189" s="2">
+        <v>200</v>
+      </c>
+      <c r="I189" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J189" s="2">
         <v>10.042726</v>
       </c>
-      <c r="K189">
+      <c r="K189" s="2">
         <v>10.042726</v>
       </c>
     </row>
-    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A190" t="s">
+    <row r="190" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B190" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C190" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D190">
+      <c r="D190" s="2">
         <v>1</v>
       </c>
-      <c r="E190">
+      <c r="E190" s="2">
         <v>10.042726</v>
       </c>
-      <c r="F190">
-        <v>200</v>
-      </c>
-      <c r="G190">
+      <c r="F190" s="2">
+        <v>200</v>
+      </c>
+      <c r="G190" s="2">
         <v>10.042726</v>
       </c>
-      <c r="H190">
-        <v>0</v>
-      </c>
-      <c r="I190" t="b">
-        <v>0</v>
-      </c>
-      <c r="J190">
-        <v>200</v>
-      </c>
-      <c r="K190">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A191" t="s">
+      <c r="H190" s="2">
+        <v>0</v>
+      </c>
+      <c r="I190" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J190" s="2">
+        <v>200</v>
+      </c>
+      <c r="K190" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C191" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D191">
+      <c r="D191" s="2">
         <v>2</v>
       </c>
-      <c r="E191">
+      <c r="E191" s="2">
         <v>10.042726</v>
       </c>
-      <c r="F191">
-        <v>0</v>
-      </c>
-      <c r="G191">
+      <c r="F191" s="2">
+        <v>0</v>
+      </c>
+      <c r="G191" s="2">
         <v>20</v>
       </c>
-      <c r="H191">
-        <v>0</v>
-      </c>
-      <c r="I191" t="b">
-        <v>0</v>
-      </c>
-      <c r="J191">
+      <c r="H191" s="2">
+        <v>0</v>
+      </c>
+      <c r="I191" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J191" s="2">
         <v>9.957274</v>
       </c>
-      <c r="K191">
+      <c r="K191" s="2">
         <v>9.957274</v>
       </c>
     </row>
-    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A192" t="s">
+    <row r="192" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C192" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D192">
+      <c r="D192" s="2">
         <v>3</v>
       </c>
-      <c r="E192">
+      <c r="E192" s="2">
         <v>20</v>
       </c>
-      <c r="F192">
-        <v>0</v>
-      </c>
-      <c r="G192">
+      <c r="F192" s="2">
+        <v>0</v>
+      </c>
+      <c r="G192" s="2">
         <v>20</v>
       </c>
-      <c r="H192">
-        <v>200</v>
-      </c>
-      <c r="I192" t="b">
-        <v>0</v>
-      </c>
-      <c r="J192">
-        <v>200</v>
-      </c>
-      <c r="K192">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="193" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A193" t="s">
+      <c r="H192" s="2">
+        <v>200</v>
+      </c>
+      <c r="I192" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J192" s="2">
+        <v>200</v>
+      </c>
+      <c r="K192" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C193" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D193">
+      <c r="D193" s="2">
         <v>4</v>
       </c>
-      <c r="E193">
+      <c r="E193" s="2">
         <v>20</v>
       </c>
-      <c r="F193">
-        <v>200</v>
-      </c>
-      <c r="G193">
+      <c r="F193" s="2">
+        <v>200</v>
+      </c>
+      <c r="G193" s="2">
         <v>10.042726</v>
       </c>
-      <c r="H193">
-        <v>200</v>
-      </c>
-      <c r="I193" t="b">
-        <v>0</v>
-      </c>
-      <c r="J193">
+      <c r="H193" s="2">
+        <v>200</v>
+      </c>
+      <c r="I193" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J193" s="2">
         <v>9.957274</v>
       </c>
-      <c r="K193">
+      <c r="K193" s="2">
         <v>9.957274</v>
       </c>
     </row>
-    <row r="194" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A194" t="s">
+    <row r="194" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C194" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D194">
+      <c r="D194" s="2">
         <v>1</v>
       </c>
-      <c r="E194">
+      <c r="E194" s="2">
         <v>10.042726</v>
       </c>
-      <c r="F194">
-        <v>0</v>
-      </c>
-      <c r="G194">
+      <c r="F194" s="2">
+        <v>0</v>
+      </c>
+      <c r="G194" s="2">
         <v>10.042726</v>
       </c>
-      <c r="H194">
-        <v>200</v>
-      </c>
-      <c r="I194" t="b">
-        <v>0</v>
-      </c>
-      <c r="J194">
-        <v>200</v>
-      </c>
-      <c r="K194">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="195" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A195" t="s">
+      <c r="H194" s="2">
+        <v>200</v>
+      </c>
+      <c r="I194" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J194" s="2">
+        <v>200</v>
+      </c>
+      <c r="K194" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C195" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D195">
+      <c r="D195" s="2">
         <v>2</v>
       </c>
-      <c r="E195">
+      <c r="E195" s="2">
         <v>10.042726</v>
       </c>
-      <c r="F195">
-        <v>200</v>
-      </c>
-      <c r="G195">
-        <v>0</v>
-      </c>
-      <c r="H195">
-        <v>200</v>
-      </c>
-      <c r="I195" t="b">
-        <v>0</v>
-      </c>
-      <c r="J195">
+      <c r="F195" s="2">
+        <v>200</v>
+      </c>
+      <c r="G195" s="2">
+        <v>0</v>
+      </c>
+      <c r="H195" s="2">
+        <v>200</v>
+      </c>
+      <c r="I195" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J195" s="2">
         <v>10.042726</v>
       </c>
-      <c r="K195">
+      <c r="K195" s="2">
         <v>10.042726</v>
       </c>
     </row>
-    <row r="196" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A196" t="s">
+    <row r="196" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B196" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C196" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D196">
+      <c r="D196" s="2">
         <v>3</v>
       </c>
-      <c r="E196">
-        <v>0</v>
-      </c>
-      <c r="F196">
-        <v>200</v>
-      </c>
-      <c r="G196">
-        <v>0</v>
-      </c>
-      <c r="H196">
-        <v>0</v>
-      </c>
-      <c r="I196" t="b">
-        <v>0</v>
-      </c>
-      <c r="J196">
-        <v>200</v>
-      </c>
-      <c r="K196">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="197" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A197" t="s">
+      <c r="E196" s="2">
+        <v>0</v>
+      </c>
+      <c r="F196" s="2">
+        <v>200</v>
+      </c>
+      <c r="G196" s="2">
+        <v>0</v>
+      </c>
+      <c r="H196" s="2">
+        <v>0</v>
+      </c>
+      <c r="I196" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J196" s="2">
+        <v>200</v>
+      </c>
+      <c r="K196" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B197" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C197" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D197">
+      <c r="D197" s="2">
         <v>4</v>
       </c>
-      <c r="E197">
-        <v>0</v>
-      </c>
-      <c r="F197">
-        <v>0</v>
-      </c>
-      <c r="G197">
+      <c r="E197" s="2">
+        <v>0</v>
+      </c>
+      <c r="F197" s="2">
+        <v>0</v>
+      </c>
+      <c r="G197" s="2">
         <v>10.042726</v>
       </c>
-      <c r="H197">
-        <v>0</v>
-      </c>
-      <c r="I197" t="b">
-        <v>0</v>
-      </c>
-      <c r="J197">
+      <c r="H197" s="2">
+        <v>0</v>
+      </c>
+      <c r="I197" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J197" s="2">
         <v>10.042726</v>
       </c>
-      <c r="K197">
+      <c r="K197" s="2">
         <v>10.042726</v>
       </c>
     </row>
-    <row r="198" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A198" t="s">
+    <row r="198" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C198" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D198">
+      <c r="D198" s="2">
         <v>1</v>
       </c>
-      <c r="E198">
-        <v>0</v>
-      </c>
-      <c r="F198">
-        <v>0</v>
-      </c>
-      <c r="G198">
+      <c r="E198" s="2">
+        <v>0</v>
+      </c>
+      <c r="F198" s="2">
+        <v>0</v>
+      </c>
+      <c r="G198" s="2">
         <v>14.204280000000001</v>
       </c>
-      <c r="H198">
-        <v>0</v>
-      </c>
-      <c r="I198" t="b">
-        <v>0</v>
-      </c>
-      <c r="J198">
+      <c r="H198" s="2">
+        <v>0</v>
+      </c>
+      <c r="I198" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J198" s="2">
         <v>14.204280000000001</v>
       </c>
-      <c r="K198">
+      <c r="K198" s="2">
         <v>14.204280000000001</v>
       </c>
-      <c r="L198">
+      <c r="L198" s="2">
         <f>K198</f>
         <v>14.204280000000001</v>
       </c>
-      <c r="M198">
+      <c r="M198" s="2">
         <v>8.0399999999999991</v>
       </c>
     </row>
-    <row r="199" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A199" t="s">
+    <row r="199" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C199" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D199">
+      <c r="D199" s="2">
         <v>2</v>
       </c>
-      <c r="E199">
+      <c r="E199" s="2">
         <v>14.204280000000001</v>
       </c>
-      <c r="F199">
-        <v>0</v>
-      </c>
-      <c r="G199">
+      <c r="F199" s="2">
+        <v>0</v>
+      </c>
+      <c r="G199" s="2">
         <v>14.204280000000001</v>
       </c>
-      <c r="H199">
-        <v>200</v>
-      </c>
-      <c r="I199" t="b">
-        <v>0</v>
-      </c>
-      <c r="J199">
-        <v>200</v>
-      </c>
-      <c r="K199">
+      <c r="H199" s="2">
+        <v>200</v>
+      </c>
+      <c r="I199" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J199" s="2">
+        <v>200</v>
+      </c>
+      <c r="K199" s="2">
         <v>14.204280000000001</v>
       </c>
     </row>
-    <row r="200" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
+    <row r="200" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C200" t="s">
+      <c r="C200" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D200">
+      <c r="D200" s="2">
         <v>3</v>
       </c>
-      <c r="E200">
+      <c r="E200" s="2">
         <v>14.204280000000001</v>
       </c>
-      <c r="F200">
-        <v>200</v>
-      </c>
-      <c r="G200">
-        <v>0</v>
-      </c>
-      <c r="H200">
-        <v>200</v>
-      </c>
-      <c r="I200" t="b">
-        <v>0</v>
-      </c>
-      <c r="J200">
+      <c r="F200" s="2">
+        <v>200</v>
+      </c>
+      <c r="G200" s="2">
+        <v>0</v>
+      </c>
+      <c r="H200" s="2">
+        <v>200</v>
+      </c>
+      <c r="I200" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J200" s="2">
         <v>14.204280000000001</v>
       </c>
-      <c r="K200">
+      <c r="K200" s="2">
         <v>14.204280000000001</v>
       </c>
     </row>
-    <row r="201" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A201" t="s">
+    <row r="201" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B201" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C201" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D201">
+      <c r="D201" s="2">
         <v>4</v>
       </c>
-      <c r="E201">
-        <v>0</v>
-      </c>
-      <c r="F201">
-        <v>200</v>
-      </c>
-      <c r="G201">
-        <v>0</v>
-      </c>
-      <c r="H201">
-        <v>0</v>
-      </c>
-      <c r="I201" t="b">
-        <v>0</v>
-      </c>
-      <c r="J201">
-        <v>200</v>
-      </c>
-      <c r="K201">
+      <c r="E201" s="2">
+        <v>0</v>
+      </c>
+      <c r="F201" s="2">
+        <v>200</v>
+      </c>
+      <c r="G201" s="2">
+        <v>0</v>
+      </c>
+      <c r="H201" s="2">
+        <v>0</v>
+      </c>
+      <c r="I201" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J201" s="2">
+        <v>200</v>
+      </c>
+      <c r="K201" s="2">
         <v>14.204280000000001</v>
       </c>
     </row>
-    <row r="202" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
+    <row r="202" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B202" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C202" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D202">
+      <c r="D202" s="2">
         <v>1</v>
       </c>
-      <c r="E202">
-        <v>0</v>
-      </c>
-      <c r="F202">
-        <v>0</v>
-      </c>
-      <c r="G202">
+      <c r="E202" s="2">
+        <v>0</v>
+      </c>
+      <c r="F202" s="2">
+        <v>0</v>
+      </c>
+      <c r="G202" s="2">
         <v>13.439035000000001</v>
       </c>
-      <c r="H202">
-        <v>0</v>
-      </c>
-      <c r="I202" t="b">
-        <v>0</v>
-      </c>
-      <c r="J202">
+      <c r="H202" s="2">
+        <v>0</v>
+      </c>
+      <c r="I202" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J202" s="2">
         <v>13.439035000000001</v>
       </c>
-      <c r="K202">
+      <c r="K202" s="2">
         <v>13.439035000000001</v>
       </c>
-      <c r="L202">
+      <c r="L202" s="2">
         <f>K202</f>
         <v>13.439035000000001</v>
       </c>
     </row>
-    <row r="203" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A203" t="s">
+    <row r="203" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A203" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B203" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C203" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D203">
+      <c r="D203" s="2">
         <v>2</v>
       </c>
-      <c r="E203">
+      <c r="E203" s="2">
         <v>13.439035000000001</v>
       </c>
-      <c r="F203">
-        <v>0</v>
-      </c>
-      <c r="G203">
+      <c r="F203" s="2">
+        <v>0</v>
+      </c>
+      <c r="G203" s="2">
         <v>13.439035000000001</v>
       </c>
-      <c r="H203">
-        <v>200</v>
-      </c>
-      <c r="I203" t="b">
-        <v>0</v>
-      </c>
-      <c r="J203">
-        <v>200</v>
-      </c>
-      <c r="K203">
+      <c r="H203" s="2">
+        <v>200</v>
+      </c>
+      <c r="I203" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J203" s="2">
+        <v>200</v>
+      </c>
+      <c r="K203" s="2">
         <v>13.439035000000001</v>
       </c>
     </row>
-    <row r="204" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A204" t="s">
+    <row r="204" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C204" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D204">
+      <c r="D204" s="2">
         <v>3</v>
       </c>
-      <c r="E204">
+      <c r="E204" s="2">
         <v>13.439035000000001</v>
       </c>
-      <c r="F204">
-        <v>200</v>
-      </c>
-      <c r="G204">
-        <v>0</v>
-      </c>
-      <c r="H204">
-        <v>200</v>
-      </c>
-      <c r="I204" t="b">
-        <v>0</v>
-      </c>
-      <c r="J204">
+      <c r="F204" s="2">
+        <v>200</v>
+      </c>
+      <c r="G204" s="2">
+        <v>0</v>
+      </c>
+      <c r="H204" s="2">
+        <v>200</v>
+      </c>
+      <c r="I204" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J204" s="2">
         <v>13.439035000000001</v>
       </c>
-      <c r="K204">
+      <c r="K204" s="2">
         <v>13.439035000000001</v>
       </c>
     </row>
-    <row r="205" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A205" t="s">
+    <row r="205" spans="1:13" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C205" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D205">
+      <c r="D205" s="2">
         <v>4</v>
       </c>
-      <c r="E205">
-        <v>0</v>
-      </c>
-      <c r="F205">
-        <v>200</v>
-      </c>
-      <c r="G205">
-        <v>0</v>
-      </c>
-      <c r="H205">
-        <v>0</v>
-      </c>
-      <c r="I205" t="b">
-        <v>0</v>
-      </c>
-      <c r="J205">
-        <v>200</v>
-      </c>
-      <c r="K205">
+      <c r="E205" s="2">
+        <v>0</v>
+      </c>
+      <c r="F205" s="2">
+        <v>200</v>
+      </c>
+      <c r="G205" s="2">
+        <v>0</v>
+      </c>
+      <c r="H205" s="2">
+        <v>0</v>
+      </c>
+      <c r="I205" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J205" s="2">
+        <v>200</v>
+      </c>
+      <c r="K205" s="2">
         <v>13.439035000000001</v>
       </c>
     </row>
@@ -8392,17 +8409,21 @@
         <v>5.9949089999999998</v>
       </c>
     </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K226">
+        <f>SUBTOTAL(9,K2:K225)</f>
+        <v>141.557863</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K225" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
-      <filters>
-        <filter val="prd.40051380.dld"/>
-      </filters>
+      <colorFilter dxfId="0"/>
     </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="ShorteningContour"/>
         <filter val="StaticComponentHull"/>
+        <filter val="VDeformableComponentHulls"/>
       </filters>
     </filterColumn>
     <filterColumn colId="3">
@@ -8412,5 +8433,20 @@
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1694A3-3069-4E96-AAC0-B9340B6311A3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>